<commit_message>
finalised file uploaded into git hub repo
</commit_message>
<xml_diff>
--- a/Website Source.xlsx
+++ b/Website Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\UWA Data Bootcamp\13. ETL-Project\ETL_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5ABEF179-459E-4DA5-9F9B-5060D66E164D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6553E3EC-31B3-4C5D-BFF6-06B25B5249C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E1906FD7-D1DF-497F-A237-2FEC0712D0CC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{E1906FD7-D1DF-497F-A237-2FEC0712D0CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Topic</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>Key Items</t>
-  </si>
-  <si>
-    <t>Chocolate Rating Scale</t>
   </si>
   <si>
     <t>https://www.kaggle.com/soroushghaderi/chocolate-bar-2020</t>
@@ -67,9 +64,6 @@
     <t xml:space="preserve">Chocolate Bean - Supply Utilization Accounts </t>
   </si>
   <si>
-    <t>Cocoa Pricing</t>
-  </si>
-  <si>
     <t>https://www.icco.org/statistics/</t>
   </si>
   <si>
@@ -79,12 +73,6 @@
     <t>https://www.kaggle.com/abishpius/global-import-of-cocoa-beans</t>
   </si>
   <si>
-    <t>Cocoa Pricing between 1970 to 2020</t>
-  </si>
-  <si>
-    <t>Cimport of Cocoa based on Region</t>
-  </si>
-  <si>
     <t>File Type</t>
   </si>
   <si>
@@ -98,6 +86,27 @@
   </si>
   <si>
     <t>csv/png</t>
+  </si>
+  <si>
+    <t>Chocolate_rating csv</t>
+  </si>
+  <si>
+    <t>Chocolate Bean - Crop livestock production</t>
+  </si>
+  <si>
+    <t>Chocolate Bean - Production Indices</t>
+  </si>
+  <si>
+    <t>Chocolate Bean - Detailed Trade Matrix</t>
+  </si>
+  <si>
+    <t>Cocoa Daily prices and Monthly Prices</t>
+  </si>
+  <si>
+    <t>Cocoa Pricing between 1994 to 2020</t>
+  </si>
+  <si>
+    <t>Import of Cocoa based on Region</t>
   </si>
 </sst>
 </file>
@@ -171,7 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -187,6 +196,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -502,16 +518,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A1EE92-D606-407E-9143-7B1E91BFA36B}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="A1:D7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85" customWidth="1"/>
     <col min="3" max="3" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -526,92 +542,134 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="B10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{8D5D536C-C93F-4C5E-9CAC-E25610387211}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{A3470544-032F-4F47-B969-5B1E66E000F3}"/>
-    <hyperlink ref="B6" r:id="rId3" xr:uid="{5F364CA8-2D1A-42D1-B212-52397F3B3151}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{A3470544-032F-4F47-B969-5B1E66E000F3}"/>
+    <hyperlink ref="B9" r:id="rId3" xr:uid="{5F364CA8-2D1A-42D1-B212-52397F3B3151}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>

</xml_diff>